<commit_message>
measurement_source_value_name에 대한 컬럼 수정
</commit_message>
<xml_diff>
--- a/JBUH/감염병_CDM_ETL정의서_20240401.xlsx
+++ b/JBUH/감염병_CDM_ETL정의서_20240401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programing\Infectious_CDM\JBUH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8B607E-A175-4A33-9FDF-AC991C983C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1368261C-E631-4176-A1D1-228276C71038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" tabRatio="855" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" tabRatio="855" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCATION" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <sheet name="PROCEDURE_OCCURRENCE" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2567,9 +2566,6 @@
 REGID</t>
   </si>
   <si>
-    <t>EXAMCODE</t>
-  </si>
-  <si>
     <t>DW_MMCUHORT
 DW_STEXMRST</t>
   </si>
@@ -2654,6 +2650,10 @@
   </si>
   <si>
     <t>ORDSEQNO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORDNAME</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3586,8 +3586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:G37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="28" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="36" t="s">
@@ -4123,7 +4123,7 @@
         <v>560</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>645</v>
+        <v>667</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="16" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
@@ -4345,23 +4345,23 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>252</v>
       </c>
       <c r="C37" s="52"/>
       <c r="D37" s="52" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F37" s="36" t="s">
         <v>560</v>
       </c>
       <c r="G37" s="52" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4429,23 +4429,23 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C41" s="52"/>
       <c r="D41" s="52" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F41" s="36" t="s">
         <v>560</v>
       </c>
       <c r="G41" s="52" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -4459,7 +4459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -4533,7 +4533,7 @@
         <v>279</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>590</v>
@@ -4577,7 +4577,7 @@
         <v>340</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>624</v>
@@ -4598,10 +4598,10 @@
         <v>350</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="17" customFormat="1" ht="54" x14ac:dyDescent="0.3">
@@ -4619,10 +4619,10 @@
         <v>351</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="17" customFormat="1" ht="27" x14ac:dyDescent="0.3">
@@ -4722,10 +4722,10 @@
         <v>406</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
@@ -4804,10 +4804,10 @@
         <v>355</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
@@ -4901,7 +4901,7 @@
         <v>442</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>620</v>
@@ -4956,7 +4956,7 @@
         <v>531</v>
       </c>
       <c r="F24" s="36" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G24" s="29" t="s">
         <v>621</v>
@@ -4977,7 +4977,7 @@
         <v>510</v>
       </c>
       <c r="F25" s="36" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G25" s="52" t="s">
         <v>596</v>
@@ -5019,7 +5019,7 @@
         <v>544</v>
       </c>
       <c r="F27" s="36" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G27" s="29" t="s">
         <v>631</v>
@@ -5040,7 +5040,7 @@
         <v>570</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G28" s="52" t="s">
         <v>624</v>
@@ -5048,107 +5048,107 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>571</v>
       </c>
       <c r="C29" s="52"/>
       <c r="D29" s="28" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F29" s="36" t="s">
         <v>540</v>
       </c>
       <c r="G29" s="52" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="27" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>252</v>
       </c>
       <c r="C30" s="52"/>
       <c r="D30" s="52" t="s">
+        <v>665</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>664</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>646</v>
+      </c>
+      <c r="G30" s="52" t="s">
         <v>666</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>665</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>647</v>
-      </c>
-      <c r="G30" s="52" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C31" s="52"/>
       <c r="D31" s="28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F31" s="36" t="s">
         <v>560</v>
       </c>
       <c r="G31" s="52" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
+        <v>648</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>649</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>650</v>
       </c>
       <c r="C32" s="52"/>
       <c r="D32" s="28" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F32" s="36" t="s">
         <v>560</v>
       </c>
       <c r="G32" s="52" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>104</v>
       </c>
       <c r="C33" s="52"/>
       <c r="D33" s="28" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F33" s="36" t="s">
         <v>560</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
   </sheetData>
@@ -5338,7 +5338,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5714,7 +5714,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A22" sqref="A22:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6374,8 +6374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6893,7 +6893,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A23" sqref="A23:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7423,7 +7423,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A22" sqref="A22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7746,7 +7746,7 @@
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="28" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>523</v>
@@ -7827,7 +7827,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>446</v>
@@ -8005,7 +8005,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="A30" sqref="A30:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8444,7 +8444,7 @@
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="28" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="36" t="s">
@@ -8828,23 +8828,23 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>252</v>
       </c>
       <c r="C40" s="52"/>
       <c r="D40" s="52" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F40" s="36" t="s">
         <v>540</v>
       </c>
       <c r="G40" s="29" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>